<commit_message>
add functionality to short custtypedetails data
</commit_message>
<xml_diff>
--- a/Data/skf_name_patterns.xlsx
+++ b/Data/skf_name_patterns.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python Code\Short-Name-Generator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7BAF40C4-573F-4D45-8F94-152DD667C13B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC0B13D-70D8-42A5-B110-05264F061EFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="skf_name_patterns" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="217">
   <si>
     <t>actual</t>
   </si>
@@ -659,12 +659,24 @@
   </si>
   <si>
     <t>Account</t>
+  </si>
+  <si>
+    <t>EMPLOYEE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Institution                                                 </t>
+  </si>
+  <si>
+    <t>Ex. HQ</t>
+  </si>
+  <si>
+    <t>Ex.HQ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -982,7 +994,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1097,6 +1109,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1142,8 +1169,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1498,16 +1526,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B127"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="C130" sqref="C130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -2526,6 +2555,46 @@
         <v>211</v>
       </c>
     </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A128" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A129" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A130" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A131" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>215</v>
+      </c>
+      <c r="B132" t="s">
+        <v>216</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Create dunamic functions suitable for multiple company
</commit_message>
<xml_diff>
--- a/Data/skf_name_patterns.xlsx
+++ b/Data/skf_name_patterns.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python Code\Short-Name-Generator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC0B13D-70D8-42A5-B110-05264F061EFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9F6773-76E2-40B7-917A-DC6A1E9BBD96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="247">
   <si>
     <t>actual</t>
   </si>
@@ -671,6 +671,96 @@
   </si>
   <si>
     <t>Ex.HQ</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>SKF</t>
+  </si>
+  <si>
+    <t>HND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">and </t>
+  </si>
+  <si>
+    <t>&amp;</t>
+  </si>
+  <si>
+    <t>Aoushadhalaya</t>
+  </si>
+  <si>
+    <t>FEED</t>
+  </si>
+  <si>
+    <t>Farm</t>
+  </si>
+  <si>
+    <t>Feed</t>
+  </si>
+  <si>
+    <t>Osadholay</t>
+  </si>
+  <si>
+    <t>Centre</t>
+  </si>
+  <si>
+    <t>Treders</t>
+  </si>
+  <si>
+    <t>Treder</t>
+  </si>
+  <si>
+    <t>Fishery</t>
+  </si>
+  <si>
+    <t>Fisharise</t>
+  </si>
+  <si>
+    <t>Fisharish</t>
+  </si>
+  <si>
+    <t>Limited</t>
+  </si>
+  <si>
+    <t>LTD</t>
+  </si>
+  <si>
+    <t>Chikishaloy</t>
+  </si>
+  <si>
+    <t>feed</t>
+  </si>
+  <si>
+    <t>Ltd.</t>
+  </si>
+  <si>
+    <t>Limited.</t>
+  </si>
+  <si>
+    <t>BD.</t>
+  </si>
+  <si>
+    <t>medical</t>
+  </si>
+  <si>
+    <t>Trader s</t>
+  </si>
+  <si>
+    <t>veterinary</t>
+  </si>
+  <si>
+    <t>Vetenirary</t>
+  </si>
+  <si>
+    <t>Co.,</t>
+  </si>
+  <si>
+    <t>Co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">And </t>
   </si>
 </sst>
 </file>
@@ -813,7 +903,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -993,6 +1083,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -1169,9 +1265,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1527,1072 +1624,3129 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B132"/>
+  <dimension ref="A1:C283"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="C130" sqref="C130"/>
+    <sheetView tabSelected="1" topLeftCell="A271" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>218</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>218</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>218</v>
+      </c>
+      <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>218</v>
+      </c>
+      <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>218</v>
+      </c>
+      <c r="B9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>218</v>
+      </c>
+      <c r="B10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>218</v>
+      </c>
+      <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>218</v>
+      </c>
+      <c r="B12" t="s">
         <v>22</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>218</v>
+      </c>
+      <c r="B13" t="s">
         <v>25</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>218</v>
+      </c>
+      <c r="B14" t="s">
         <v>27</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>218</v>
+      </c>
+      <c r="B15" t="s">
         <v>29</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>218</v>
+      </c>
+      <c r="B16" t="s">
         <v>31</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>218</v>
+      </c>
+      <c r="B17" t="s">
         <v>33</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
+        <v>218</v>
+      </c>
+      <c r="B18" t="s">
         <v>35</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>218</v>
+      </c>
+      <c r="B19" t="s">
         <v>36</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
+        <v>218</v>
+      </c>
+      <c r="B20" t="s">
         <v>38</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
+        <v>218</v>
+      </c>
+      <c r="B21" t="s">
         <v>40</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
+        <v>218</v>
+      </c>
+      <c r="B22" t="s">
         <v>42</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>218</v>
+      </c>
+      <c r="B23" t="s">
         <v>44</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>218</v>
+      </c>
+      <c r="B24" t="s">
         <v>45</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
+        <v>218</v>
+      </c>
+      <c r="B25" t="s">
         <v>46</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
+        <v>218</v>
+      </c>
+      <c r="B26" t="s">
         <v>46</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
+        <v>218</v>
+      </c>
+      <c r="B27" t="s">
         <v>48</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
+        <v>218</v>
+      </c>
+      <c r="B28" t="s">
         <v>50</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
+        <v>218</v>
+      </c>
+      <c r="B29" t="s">
         <v>52</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>218</v>
+      </c>
+      <c r="B30" t="s">
         <v>54</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
+        <v>218</v>
+      </c>
+      <c r="B31" t="s">
         <v>56</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
+        <v>218</v>
+      </c>
+      <c r="B32" t="s">
         <v>58</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
+        <v>218</v>
+      </c>
+      <c r="B33" t="s">
         <v>60</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
+        <v>218</v>
+      </c>
+      <c r="B34" t="s">
         <v>61</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
+        <v>218</v>
+      </c>
+      <c r="B35" t="s">
         <v>63</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
+        <v>218</v>
+      </c>
+      <c r="B36" t="s">
         <v>64</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
+        <v>218</v>
+      </c>
+      <c r="B37" t="s">
         <v>66</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
+        <v>218</v>
+      </c>
+      <c r="B38" t="s">
         <v>68</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
+        <v>218</v>
+      </c>
+      <c r="B39" t="s">
         <v>70</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
+        <v>218</v>
+      </c>
+      <c r="B40" t="s">
         <v>71</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
+        <v>218</v>
+      </c>
+      <c r="B41" t="s">
         <v>73</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
+        <v>218</v>
+      </c>
+      <c r="B42" t="s">
         <v>75</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
+        <v>218</v>
+      </c>
+      <c r="B43" t="s">
         <v>77</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
+        <v>218</v>
+      </c>
+      <c r="B44" t="s">
         <v>79</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
+        <v>218</v>
+      </c>
+      <c r="B45" t="s">
         <v>81</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
+        <v>218</v>
+      </c>
+      <c r="B46" t="s">
         <v>82</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
+        <v>218</v>
+      </c>
+      <c r="B47" t="s">
         <v>84</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
+        <v>218</v>
+      </c>
+      <c r="B48" t="s">
         <v>86</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
+        <v>218</v>
+      </c>
+      <c r="B49" t="s">
         <v>88</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
+        <v>218</v>
+      </c>
+      <c r="B50" t="s">
         <v>89</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
+        <v>218</v>
+      </c>
+      <c r="B51" t="s">
         <v>91</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
+        <v>218</v>
+      </c>
+      <c r="B52" t="s">
         <v>93</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
+        <v>218</v>
+      </c>
+      <c r="B53" t="s">
         <v>95</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
+        <v>218</v>
+      </c>
+      <c r="B54" t="s">
         <v>97</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
+        <v>218</v>
+      </c>
+      <c r="B55" t="s">
         <v>99</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
+        <v>218</v>
+      </c>
+      <c r="B56" t="s">
         <v>101</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
+        <v>218</v>
+      </c>
+      <c r="B57" t="s">
         <v>103</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C57" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
+        <v>218</v>
+      </c>
+      <c r="B58" t="s">
         <v>105</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
+        <v>218</v>
+      </c>
+      <c r="B59" t="s">
         <v>107</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
+        <v>218</v>
+      </c>
+      <c r="B60" t="s">
         <v>109</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C60" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
+        <v>218</v>
+      </c>
+      <c r="B61" t="s">
         <v>111</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
+        <v>218</v>
+      </c>
+      <c r="B62" t="s">
         <v>113</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
+        <v>218</v>
+      </c>
+      <c r="B63" t="s">
         <v>115</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
+        <v>218</v>
+      </c>
+      <c r="B64" t="s">
         <v>117</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
+        <v>218</v>
+      </c>
+      <c r="B65" t="s">
         <v>119</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
+        <v>218</v>
+      </c>
+      <c r="B66" t="s">
         <v>120</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
+        <v>218</v>
+      </c>
+      <c r="B67" t="s">
         <v>121</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
+        <v>218</v>
+      </c>
+      <c r="B68" t="s">
         <v>117</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
+        <v>218</v>
+      </c>
+      <c r="B69" t="s">
         <v>122</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
+        <v>218</v>
+      </c>
+      <c r="B70" t="s">
         <v>124</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
+        <v>218</v>
+      </c>
+      <c r="B71" t="s">
         <v>126</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C71" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
+        <v>218</v>
+      </c>
+      <c r="B72" t="s">
         <v>128</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C72" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
+        <v>218</v>
+      </c>
+      <c r="B73" t="s">
         <v>130</v>
       </c>
-      <c r="B73" t="s">
+      <c r="C73" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
+        <v>218</v>
+      </c>
+      <c r="B74" t="s">
         <v>132</v>
       </c>
-      <c r="B74" t="s">
+      <c r="C74" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
+        <v>218</v>
+      </c>
+      <c r="B75" t="s">
         <v>134</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C75" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
+        <v>218</v>
+      </c>
+      <c r="B76" t="s">
         <v>136</v>
       </c>
-      <c r="B76" t="s">
+      <c r="C76" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
+        <v>218</v>
+      </c>
+      <c r="B77" t="s">
         <v>137</v>
       </c>
-      <c r="B77" t="s">
+      <c r="C77" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
+        <v>218</v>
+      </c>
+      <c r="B78" t="s">
         <v>139</v>
       </c>
-      <c r="B78" t="s">
+      <c r="C78" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
+        <v>218</v>
+      </c>
+      <c r="B79" t="s">
         <v>141</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C79" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
+        <v>218</v>
+      </c>
+      <c r="B80" t="s">
         <v>143</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C80" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
+        <v>218</v>
+      </c>
+      <c r="B81" t="s">
         <v>145</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C81" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
+        <v>218</v>
+      </c>
+      <c r="B82" t="s">
         <v>147</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C82" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
+        <v>218</v>
+      </c>
+      <c r="B83" t="s">
         <v>149</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C83" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
+        <v>218</v>
+      </c>
+      <c r="B84" t="s">
         <v>151</v>
       </c>
-      <c r="B84" t="s">
+      <c r="C84" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
+        <v>218</v>
+      </c>
+      <c r="B85" t="s">
         <v>153</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C85" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
+        <v>218</v>
+      </c>
+      <c r="B86" t="s">
         <v>154</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C86" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
+        <v>218</v>
+      </c>
+      <c r="B87" t="s">
         <v>156</v>
       </c>
-      <c r="B87" t="s">
+      <c r="C87" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
+        <v>218</v>
+      </c>
+      <c r="B88" t="s">
         <v>157</v>
       </c>
-      <c r="B88" t="s">
+      <c r="C88" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
+        <v>218</v>
+      </c>
+      <c r="B89" t="s">
         <v>158</v>
       </c>
-      <c r="B89" t="s">
+      <c r="C89" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
+        <v>218</v>
+      </c>
+      <c r="B90" t="s">
         <v>160</v>
       </c>
-      <c r="B90" t="s">
+      <c r="C90" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
+        <v>218</v>
+      </c>
+      <c r="B91" t="s">
         <v>162</v>
       </c>
-      <c r="B91" t="s">
+      <c r="C91" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
+        <v>218</v>
+      </c>
+      <c r="B92" t="s">
         <v>164</v>
       </c>
-      <c r="B92" t="s">
+      <c r="C92" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
+        <v>218</v>
+      </c>
+      <c r="B93" t="s">
         <v>166</v>
       </c>
-      <c r="B93" t="s">
+      <c r="C93" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
+        <v>218</v>
+      </c>
+      <c r="B94" t="s">
         <v>168</v>
       </c>
-      <c r="B94" t="s">
+      <c r="C94" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
+        <v>218</v>
+      </c>
+      <c r="B95" t="s">
         <v>170</v>
       </c>
-      <c r="B95" t="s">
+      <c r="C95" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
+        <v>218</v>
+      </c>
+      <c r="B96" t="s">
         <v>170</v>
       </c>
-      <c r="B96" t="s">
+      <c r="C96" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
+        <v>218</v>
+      </c>
+      <c r="B97" t="s">
         <v>171</v>
       </c>
-      <c r="B97" t="s">
+      <c r="C97" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
+        <v>218</v>
+      </c>
+      <c r="B98" t="s">
         <v>173</v>
       </c>
-      <c r="B98" t="s">
+      <c r="C98" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
+        <v>218</v>
+      </c>
+      <c r="B99" t="s">
         <v>175</v>
       </c>
-      <c r="B99" t="s">
+      <c r="C99" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
+        <v>218</v>
+      </c>
+      <c r="B100" t="s">
         <v>177</v>
       </c>
-      <c r="B100" t="s">
+      <c r="C100" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
+        <v>218</v>
+      </c>
+      <c r="B101" t="s">
         <v>179</v>
       </c>
-      <c r="B101" t="s">
+      <c r="C101" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
+        <v>218</v>
+      </c>
+      <c r="B102" t="s">
         <v>181</v>
       </c>
-      <c r="B102" t="s">
+      <c r="C102" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
+        <v>218</v>
+      </c>
+      <c r="B103" t="s">
         <v>183</v>
       </c>
-      <c r="B103" t="s">
+      <c r="C103" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
+        <v>218</v>
+      </c>
+      <c r="B104" t="s">
         <v>185</v>
       </c>
-      <c r="B104" t="s">
+      <c r="C104" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
+        <v>218</v>
+      </c>
+      <c r="B105" t="s">
         <v>187</v>
       </c>
-      <c r="B105" t="s">
+      <c r="C105" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
+        <v>218</v>
+      </c>
+      <c r="B106" t="s">
         <v>188</v>
       </c>
-      <c r="B106" t="s">
+      <c r="C106" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
+        <v>218</v>
+      </c>
+      <c r="B107" t="s">
         <v>190</v>
       </c>
-      <c r="B107" t="s">
+      <c r="C107" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
+        <v>218</v>
+      </c>
+      <c r="B108" t="s">
         <v>192</v>
       </c>
-      <c r="B108" t="s">
+      <c r="C108" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
+        <v>218</v>
+      </c>
+      <c r="B109" t="s">
         <v>193</v>
       </c>
-      <c r="B109" t="s">
+      <c r="C109" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
+        <v>218</v>
+      </c>
+      <c r="B110" t="s">
         <v>195</v>
       </c>
-      <c r="B110" t="s">
+      <c r="C110" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
+        <v>218</v>
+      </c>
+      <c r="B111" t="s">
         <v>196</v>
       </c>
-      <c r="B111" t="s">
+      <c r="C111" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
+        <v>218</v>
+      </c>
+      <c r="B112" t="s">
         <v>197</v>
       </c>
-      <c r="B112" t="s">
+      <c r="C112" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
+        <v>218</v>
+      </c>
+      <c r="B113" t="s">
         <v>128</v>
       </c>
-      <c r="B113" t="s">
+      <c r="C113" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
+        <v>218</v>
+      </c>
+      <c r="B114" t="s">
         <v>156</v>
       </c>
-      <c r="B114" t="s">
+      <c r="C114" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
+        <v>218</v>
+      </c>
+      <c r="B115" t="s">
         <v>198</v>
       </c>
-      <c r="B115" t="s">
+      <c r="C115" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
+        <v>218</v>
+      </c>
+      <c r="B116" t="s">
         <v>199</v>
       </c>
-      <c r="B116" t="s">
+      <c r="C116" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
+        <v>218</v>
+      </c>
+      <c r="B117" t="s">
         <v>200</v>
       </c>
-      <c r="B117" t="s">
+      <c r="C117" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
+        <v>218</v>
+      </c>
+      <c r="B118" t="s">
         <v>201</v>
       </c>
-      <c r="B118" t="s">
+      <c r="C118" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
+        <v>218</v>
+      </c>
+      <c r="B119" t="s">
         <v>202</v>
       </c>
-      <c r="B119" t="s">
+      <c r="C119" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
+        <v>218</v>
+      </c>
+      <c r="B120" t="s">
         <v>203</v>
       </c>
-      <c r="B120" t="s">
+      <c r="C120" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
+        <v>218</v>
+      </c>
+      <c r="B121" t="s">
         <v>204</v>
       </c>
-      <c r="B121" t="s">
+      <c r="C121" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
+        <v>218</v>
+      </c>
+      <c r="B122" t="s">
         <v>205</v>
       </c>
-      <c r="B122" t="s">
+      <c r="C122" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
+        <v>218</v>
+      </c>
+      <c r="B123" t="s">
         <v>206</v>
       </c>
-      <c r="B123" t="s">
+      <c r="C123" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
+        <v>218</v>
+      </c>
+      <c r="B124" t="s">
         <v>208</v>
       </c>
-      <c r="B124" t="s">
+      <c r="C124" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
+        <v>218</v>
+      </c>
+      <c r="B125" t="s">
         <v>209</v>
       </c>
-      <c r="B125" t="s">
+      <c r="C125" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
+        <v>218</v>
+      </c>
+      <c r="B126" t="s">
         <v>210</v>
       </c>
-      <c r="B126" t="s">
+      <c r="C126" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
+        <v>218</v>
+      </c>
+      <c r="B127" t="s">
         <v>212</v>
       </c>
-      <c r="B127" t="s">
+      <c r="C127" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A128" s="1" t="s">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>218</v>
+      </c>
+      <c r="B128" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B128" s="1" t="s">
+      <c r="C128" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A129" s="1" t="s">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>218</v>
+      </c>
+      <c r="B129" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B129" s="1" t="s">
+      <c r="C129" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A130" s="1" t="s">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>218</v>
+      </c>
+      <c r="B130" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B130" s="1" t="s">
+      <c r="C130" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A131" s="1" t="s">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>218</v>
+      </c>
+      <c r="B131" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B131" s="1" t="s">
+      <c r="C131" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
+        <v>218</v>
+      </c>
+      <c r="B132" t="s">
         <v>215</v>
       </c>
-      <c r="B132" t="s">
+      <c r="C132" t="s">
         <v>216</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>219</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>219</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>219</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>219</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>219</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>219</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>219</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>219</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>219</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>219</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>219</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>219</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>219</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>219</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>219</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>219</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>219</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
+        <v>219</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>219</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>219</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
+        <v>219</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
+        <v>219</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
+        <v>219</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
+        <v>219</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A157" t="s">
+        <v>219</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A158" t="s">
+        <v>219</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A159" t="s">
+        <v>219</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
+        <v>219</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
+        <v>219</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
+        <v>219</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A163" t="s">
+        <v>219</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A164" t="s">
+        <v>219</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A165" t="s">
+        <v>219</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A166" t="s">
+        <v>219</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A167" t="s">
+        <v>219</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A168" t="s">
+        <v>219</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A169" t="s">
+        <v>219</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A170" t="s">
+        <v>219</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A171" t="s">
+        <v>219</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A172" t="s">
+        <v>219</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C172" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A173" t="s">
+        <v>219</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C173" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A174" t="s">
+        <v>219</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A175" t="s">
+        <v>219</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A176" t="s">
+        <v>219</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A177" t="s">
+        <v>219</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A178" t="s">
+        <v>219</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A179" t="s">
+        <v>219</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A180" t="s">
+        <v>219</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A181" t="s">
+        <v>219</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A182" t="s">
+        <v>219</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A183" t="s">
+        <v>219</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C183" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A184" t="s">
+        <v>219</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A185" t="s">
+        <v>219</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A186" t="s">
+        <v>219</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C186" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A187" t="s">
+        <v>219</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C187" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A188" t="s">
+        <v>219</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C188" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A189" t="s">
+        <v>219</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A190" t="s">
+        <v>219</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A191" t="s">
+        <v>219</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A192" t="s">
+        <v>219</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A193" t="s">
+        <v>219</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A194" t="s">
+        <v>219</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C194" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A195" t="s">
+        <v>219</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C195" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A196" t="s">
+        <v>219</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A197" t="s">
+        <v>219</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C197" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A198" t="s">
+        <v>219</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C198" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A199" t="s">
+        <v>219</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A200" t="s">
+        <v>219</v>
+      </c>
+      <c r="B200" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A201" t="s">
+        <v>219</v>
+      </c>
+      <c r="B201" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C201" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A202" t="s">
+        <v>219</v>
+      </c>
+      <c r="B202" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A203" t="s">
+        <v>219</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A204" t="s">
+        <v>219</v>
+      </c>
+      <c r="B204" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C204" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A205" t="s">
+        <v>219</v>
+      </c>
+      <c r="B205" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C205" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A206" t="s">
+        <v>219</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C206" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A207" t="s">
+        <v>219</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A208" t="s">
+        <v>219</v>
+      </c>
+      <c r="B208" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C208" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A209" t="s">
+        <v>219</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C209" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A210" t="s">
+        <v>219</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C210" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A211" t="s">
+        <v>219</v>
+      </c>
+      <c r="B211" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C211" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A212" t="s">
+        <v>219</v>
+      </c>
+      <c r="B212" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C212" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A213" t="s">
+        <v>219</v>
+      </c>
+      <c r="B213" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C213" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A214" t="s">
+        <v>219</v>
+      </c>
+      <c r="B214" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C214" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A215" t="s">
+        <v>219</v>
+      </c>
+      <c r="B215" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C215" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A216" t="s">
+        <v>219</v>
+      </c>
+      <c r="B216" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C216" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A217" t="s">
+        <v>219</v>
+      </c>
+      <c r="B217" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C217" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A218" t="s">
+        <v>219</v>
+      </c>
+      <c r="B218" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C218" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A219" t="s">
+        <v>219</v>
+      </c>
+      <c r="B219" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C219" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A220" t="s">
+        <v>219</v>
+      </c>
+      <c r="B220" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C220" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A221" t="s">
+        <v>219</v>
+      </c>
+      <c r="B221" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C221" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A222" t="s">
+        <v>219</v>
+      </c>
+      <c r="B222" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C222" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A223" t="s">
+        <v>219</v>
+      </c>
+      <c r="B223" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A224" t="s">
+        <v>219</v>
+      </c>
+      <c r="B224" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A225" t="s">
+        <v>219</v>
+      </c>
+      <c r="B225" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C225" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A226" t="s">
+        <v>219</v>
+      </c>
+      <c r="B226" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C226" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A227" t="s">
+        <v>219</v>
+      </c>
+      <c r="B227" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A228" t="s">
+        <v>219</v>
+      </c>
+      <c r="B228" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A229" t="s">
+        <v>219</v>
+      </c>
+      <c r="B229" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C229" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A230" t="s">
+        <v>219</v>
+      </c>
+      <c r="B230" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A231" t="s">
+        <v>219</v>
+      </c>
+      <c r="B231" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C231" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A232" t="s">
+        <v>219</v>
+      </c>
+      <c r="B232" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C232" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A233" t="s">
+        <v>219</v>
+      </c>
+      <c r="B233" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C233" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A234" t="s">
+        <v>219</v>
+      </c>
+      <c r="B234" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C234" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A235" t="s">
+        <v>219</v>
+      </c>
+      <c r="B235" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C235" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A236" t="s">
+        <v>219</v>
+      </c>
+      <c r="B236" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C236" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A237" t="s">
+        <v>219</v>
+      </c>
+      <c r="B237" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C237" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A238" t="s">
+        <v>219</v>
+      </c>
+      <c r="B238" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C238" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A239" t="s">
+        <v>219</v>
+      </c>
+      <c r="B239" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C239" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A240" t="s">
+        <v>219</v>
+      </c>
+      <c r="B240" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C240" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A241" t="s">
+        <v>219</v>
+      </c>
+      <c r="B241" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C241" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A242" t="s">
+        <v>219</v>
+      </c>
+      <c r="B242" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C242" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A243" t="s">
+        <v>219</v>
+      </c>
+      <c r="B243" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C243" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A244" t="s">
+        <v>219</v>
+      </c>
+      <c r="B244" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C244" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A245" t="s">
+        <v>219</v>
+      </c>
+      <c r="B245" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C245" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A246" t="s">
+        <v>219</v>
+      </c>
+      <c r="B246" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C246" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A247" t="s">
+        <v>219</v>
+      </c>
+      <c r="B247" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C247" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A248" t="s">
+        <v>219</v>
+      </c>
+      <c r="B248" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C248" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A249" t="s">
+        <v>219</v>
+      </c>
+      <c r="B249" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C249" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A250" t="s">
+        <v>219</v>
+      </c>
+      <c r="B250" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C250" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A251" t="s">
+        <v>219</v>
+      </c>
+      <c r="B251" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C251" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A252" t="s">
+        <v>219</v>
+      </c>
+      <c r="B252" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C252" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A253" t="s">
+        <v>219</v>
+      </c>
+      <c r="B253" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C253" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A254" t="s">
+        <v>219</v>
+      </c>
+      <c r="B254" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C254" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A255" t="s">
+        <v>219</v>
+      </c>
+      <c r="B255" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C255" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A256" t="s">
+        <v>219</v>
+      </c>
+      <c r="B256" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C256" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A257" t="s">
+        <v>219</v>
+      </c>
+      <c r="B257" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C257" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A258" t="s">
+        <v>219</v>
+      </c>
+      <c r="B258" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C258" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A259" t="s">
+        <v>219</v>
+      </c>
+      <c r="B259" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C259" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A260" t="s">
+        <v>219</v>
+      </c>
+      <c r="B260" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C260" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A261" t="s">
+        <v>219</v>
+      </c>
+      <c r="B261" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C261" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A262" t="s">
+        <v>219</v>
+      </c>
+      <c r="B262" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C262" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A263" t="s">
+        <v>219</v>
+      </c>
+      <c r="B263" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C263" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A264" t="s">
+        <v>219</v>
+      </c>
+      <c r="B264" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C264" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A265" t="s">
+        <v>219</v>
+      </c>
+      <c r="B265" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C265" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A266" t="s">
+        <v>219</v>
+      </c>
+      <c r="B266" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C266" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A267" t="s">
+        <v>219</v>
+      </c>
+      <c r="B267" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C267" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A268" t="s">
+        <v>219</v>
+      </c>
+      <c r="B268" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C268" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A269" t="s">
+        <v>219</v>
+      </c>
+      <c r="B269" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C269" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A270" t="s">
+        <v>219</v>
+      </c>
+      <c r="B270" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C270" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A271" t="s">
+        <v>219</v>
+      </c>
+      <c r="B271" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C271" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A272" t="s">
+        <v>219</v>
+      </c>
+      <c r="B272" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C272" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A273" t="s">
+        <v>219</v>
+      </c>
+      <c r="B273" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C273" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A274" t="s">
+        <v>219</v>
+      </c>
+      <c r="B274" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C274" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A275" t="s">
+        <v>219</v>
+      </c>
+      <c r="B275" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C275" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A276" t="s">
+        <v>219</v>
+      </c>
+      <c r="B276" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C276" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A277" t="s">
+        <v>219</v>
+      </c>
+      <c r="B277" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C277" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A278" t="s">
+        <v>219</v>
+      </c>
+      <c r="B278" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C278" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A279" t="s">
+        <v>219</v>
+      </c>
+      <c r="B279" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C279" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A280" t="s">
+        <v>219</v>
+      </c>
+      <c r="B280" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C280" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A281" t="s">
+        <v>219</v>
+      </c>
+      <c r="B281" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C281" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A282" t="s">
+        <v>219</v>
+      </c>
+      <c r="B282" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C282" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A283" t="s">
+        <v>219</v>
+      </c>
+      <c r="B283" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C283" s="2" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>